<commit_message>
1. added code for the proximity search model
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,33 +20,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">STEMMED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uninterpolated MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision at 10 docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision at 30 docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TF-IDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okapi BM25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unigram LM with Laplace smoothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
+  </si>
   <si>
     <t xml:space="preserve">NON STEMMED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uninterpolated MAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precision at 10 docs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precision at 30 docs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TF-IDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Okapi BM25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unigram LM with Laplace smoothing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,7 +348,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added results and updated the summary spreadsheets
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t xml:space="preserve">STEMMED</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Unigram LM with Laplace smoothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity Search</t>
   </si>
   <si>
     <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
@@ -224,10 +227,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,159 +302,215 @@
         <v>0.2907</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>0.2886</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.396</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.3293</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>0.2901</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0.3507</v>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.2933</v>
+        <v>0.2901</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.428</v>
+        <v>0.416</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.332</v>
+        <v>0.3507</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.2933</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0.332</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B11" s="0" t="n">
         <v>0.1952</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C11" s="0" t="n">
         <v>0.388</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D11" s="0" t="n">
         <v>0.3053</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.2932</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.3293</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.1491</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0.2027</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>0.1544</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>0.2027</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.1491</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.1544</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B18" s="0" t="n">
         <v>0.1041</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C18" s="0" t="n">
         <v>0.224</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>0.1707</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.1544</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B22" s="0" t="n">
         <v>0.1546</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C22" s="0" t="n">
         <v>0.244</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D22" s="0" t="n">
         <v>0.2053</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B23" s="0" t="n">
         <v>0.1605</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C23" s="0" t="n">
         <v>0.268</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <v>0.2053</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B24" s="0" t="n">
         <v>0.1079</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C24" s="0" t="n">
         <v>0.224</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <v>0.172</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.1605</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.268</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.2053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. adding results for proximity search for unmodified queries 2. making the no ops compressor as a default one
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
     <t xml:space="preserve">STEMMED</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity Search (Unmodified queries)</t>
   </si>
   <si>
     <t xml:space="preserve">NON STEMMED</t>
@@ -227,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,48 +380,48 @@
         <v>0.3293</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.2194</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.2827</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>0.1491</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>0.2027</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.1544</v>
+        <v>0.1491</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.26</v>
+        <v>0.244</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.2027</v>
@@ -426,60 +429,60 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.1041</v>
+        <v>0.1544</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.224</v>
+        <v>0.26</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.1707</v>
+        <v>0.2027</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.1041</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0.1707</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B20" s="0" t="n">
         <v>0.1544</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C20" s="0" t="n">
         <v>0.26</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D20" s="0" t="n">
         <v>0.2027</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>0.1546</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>0.2053</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.1605</v>
+        <v>0.1546</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.268</v>
+        <v>0.244</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.2053</v>
@@ -487,29 +490,43 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.1079</v>
+        <v>0.1605</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.224</v>
+        <v>0.268</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.172</v>
+        <v>0.2053</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.1079</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.172</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B26" s="0" t="n">
         <v>0.1605</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C26" s="0" t="n">
         <v>0.268</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <v>0.2053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added size of indexes as well to the summary
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,7 +20,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">INDEX TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressed Stemmed Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressed Stemmed Head Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressed Non Stemmed Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressed Non Stemmed Head Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Stemmed Text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Raw </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Stemmed Head Text</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Raw </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Non Stemmed Text</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Raw </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Non Stemmed Head Text</t>
+    </r>
+  </si>
   <si>
     <t xml:space="preserve">STEMMED</t>
   </si>
@@ -65,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -95,13 +173,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5E8AC7"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -144,12 +233,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,7 +276,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF5E8AC7"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -230,10 +327,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -248,285 +345,357 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+      <c r="B2" s="0" t="n">
+        <v>84.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.2856</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.404</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0.3387</v>
+        <v>86.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.2888</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.404</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.332</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>91.3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0.1912</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0.384</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0.2907</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B8" s="0" t="n">
+        <v>194.3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0.2886</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.396</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.3293</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="0" t="n">
+        <v>196.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>0.2901</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0.416</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>0.3507</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="B10" s="0" t="n">
-        <v>0.2933</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.428</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>201.6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.2856</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.3387</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.2888</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0.404</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>0.332</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>0.1952</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>0.388</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>0.3053</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>0.2932</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>0.424</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>0.3293</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0.2194</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0.2827</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.1491</v>
+        <v>0.1912</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.244</v>
+        <v>0.384</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.2027</v>
+        <v>0.2907</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.1544</v>
+        <v>0.2886</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.26</v>
+        <v>0.396</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.2027</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0.1041</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0.224</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>0.1707</v>
+        <v>0.3293</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>0.1544</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>0.2027</v>
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.2901</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0.3507</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>9</v>
+      <c r="A22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0.2933</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>0.332</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.1546</v>
+        <v>0.1952</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.244</v>
+        <v>0.388</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>0.2053</v>
+        <v>0.3053</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0.1605</v>
+        <v>0.2932</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.268</v>
+        <v>0.424</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>0.2053</v>
+        <v>0.3293</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B25" s="0" t="n">
+        <v>0.2194</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>0.2827</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.1491</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.1544</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0.1041</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.1707</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.1544</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.2027</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.1546</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0.2053</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.1605</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0.268</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0.2053</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="0" t="n">
         <v>0.1079</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C37" s="0" t="n">
         <v>0.224</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D37" s="0" t="n">
         <v>0.172</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="0" t="n">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="0" t="n">
         <v>0.1605</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C38" s="0" t="n">
         <v>0.268</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D38" s="0" t="n">
         <v>0.2053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the summary for the proximity search
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t xml:space="preserve">INDEX TYPE</t>
   </si>
@@ -43,61 +43,13 @@
     <t xml:space="preserve">Raw Stemmed Text</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Raw </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Stemmed Head Text</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Raw </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Non Stemmed Text</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Raw </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Non Stemmed Head Text</t>
-    </r>
+    <t xml:space="preserve">Raw Stemmed Head Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Non Stemmed Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw Non Stemmed Head Text</t>
   </si>
   <si>
     <t xml:space="preserve">STEMMED</t>
@@ -124,13 +76,13 @@
     <t xml:space="preserve">Unigram LM with Laplace smoothing</t>
   </si>
   <si>
+    <t xml:space="preserve">Proximity Search (Unmodified queries)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Proximity Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximity Search (Unmodified queries)</t>
   </si>
   <si>
     <t xml:space="preserve">NON STEMMED</t>
@@ -143,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -172,11 +124,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -242,7 +189,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,10 +274,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,13 +426,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>0.2886</v>
+        <v>0.2354</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.396</v>
+        <v>0.36</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.3293</v>
+        <v>0.2907</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +484,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.2932</v>
@@ -549,48 +496,48 @@
         <v>0.3293</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>0.2194</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0.2827</v>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>14</v>
+      <c r="A28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.1491</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.2027</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>0.1491</v>
+        <v>0.1544</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0.244</v>
+        <v>0.26</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>0.2027</v>
@@ -598,60 +545,60 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0.1544</v>
+        <v>0.1041</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0.26</v>
+        <v>0.224</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>0.2027</v>
+        <v>0.1707</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.1041</v>
+        <v>0.1842</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0.224</v>
+        <v>0.272</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>0.1707</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>0.1544</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>0.2027</v>
+        <v>0.2347</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>19</v>
+      <c r="A34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0.1546</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0.2053</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.1546</v>
+        <v>0.1605</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>0.244</v>
+        <v>0.268</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>0.2053</v>
@@ -659,43 +606,29 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>0.1605</v>
+        <v>0.1079</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.268</v>
+        <v>0.224</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>0.2053</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.1079</v>
+        <v>0.1605</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0.224</v>
+        <v>0.268</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>0.172</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>0.1605</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>0.268</v>
-      </c>
-      <c r="D38" s="0" t="n">
         <v>0.2053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added results for jelinek mercer and updated the summary for the same
</commit_message>
<xml_diff>
--- a/HW_2/Summary.xlsx
+++ b/HW_2/Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t xml:space="preserve">INDEX TYPE</t>
   </si>
@@ -73,13 +73,16 @@
     <t xml:space="preserve">Okapi BM25</t>
   </si>
   <si>
+    <t xml:space="preserve">Unigram LM with Jelinek-Mercer smoothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximity Search (Unmodified queries)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unigram LM with Laplace smoothing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proximity Search (Unmodified queries)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">With HEAD – TEXT Indexed EC2</t>
   </si>
   <si>
     <t xml:space="preserve">Proximity Search</t>
@@ -277,7 +280,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -412,13 +415,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>0.1912</v>
+        <v>0.2301</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.384</v>
+        <v>0.344</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>0.2907</v>
+        <v>0.2787</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,7 +473,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.1952</v>
@@ -484,7 +487,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.2932</v>
@@ -498,7 +501,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,7 +548,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.1041</v>
@@ -606,7 +609,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0.1079</v>
@@ -620,7 +623,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.1605</v>

</xml_diff>